<commit_message>
K value for spherical magnet
</commit_message>
<xml_diff>
--- a/Software/K Values for Multiple Magnets.xlsx
+++ b/Software/K Values for Multiple Magnets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd3dlab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd3dlab\Documents\Github\AugmentedStethoscope\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>x</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Taking Entire Norm</t>
+  </si>
+  <si>
+    <t>SPEHRICAL MAGNET</t>
   </si>
 </sst>
 </file>
@@ -338,6 +341,14 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -347,9 +358,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -359,20 +367,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,298 +669,444 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="2">
         <v>6.86</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C6" si="0">A3*B3^6</f>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C5" si="0">A3*B3^6</f>
         <v>1.2209326171874999E-6</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="4">
+      <c r="D3" s="13"/>
+      <c r="E3" s="1">
         <f>2.61^2</f>
         <v>6.8120999999999992</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G3" s="6">
-        <f t="shared" ref="G3:G6" si="1">E3*F3^6</f>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="1">E3*F3^6</f>
         <v>1.2124074462890622E-6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="2">
         <v>2.87</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>1.0824191098437507E-6</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="4">
+      <c r="D4" s="13"/>
+      <c r="E4" s="1">
         <f>1.69^2</f>
         <v>2.8560999999999996</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="1">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="3">
         <f t="shared" si="1"/>
         <v>1.0771767315765628E-6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="2">
         <v>1.31</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>9.6297037671875006E-7</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="4">
+      <c r="D5" s="13"/>
+      <c r="E5" s="1">
         <f>1.13^2</f>
         <v>1.2768999999999997</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="3">
         <f t="shared" si="1"/>
         <v>9.3863883513906222E-7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="6"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="13">
+      <c r="B8" s="16"/>
+      <c r="C8" s="7">
         <f>AVERAGE(C3:C5)</f>
         <v>1.0887740345833337E-6</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="16" t="s">
+      <c r="D8" s="14"/>
+      <c r="E8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="17">
+      <c r="F8" s="16"/>
+      <c r="G8" s="8">
         <f>AVERAGE(G3:G5)</f>
         <v>1.0760743376682291E-6</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="11" t="s">
+      <c r="D11" s="12"/>
+      <c r="E11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="2">
         <v>0.755</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C12" s="4">
-        <f t="shared" ref="C12:C15" si="2">A12*B12^6</f>
+      <c r="C12" s="1">
+        <f t="shared" ref="C12:C14" si="2">A12*B12^6</f>
         <v>1.3437377929687499E-7</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="4">
+      <c r="D12" s="13"/>
+      <c r="E12" s="1">
         <f>0.863^2</f>
         <v>0.74476900000000001</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G12" s="6">
-        <f t="shared" ref="G12:G15" si="3">E12*F12^6</f>
+      <c r="G12" s="3">
+        <f t="shared" ref="G12:G14" si="3">E12*F12^6</f>
         <v>1.3255288110351561E-7</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="2">
         <v>0.41</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="1">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="1">
         <f t="shared" si="2"/>
         <v>1.5463130140625006E-7</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="4">
+      <c r="D13" s="13"/>
+      <c r="E13" s="1">
         <f>0.639^2</f>
         <v>0.40832099999999999</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="1">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="3">
         <f t="shared" si="3"/>
         <v>1.5399806736951569E-7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="2">
         <v>0.27500000000000002</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="1">
         <f t="shared" si="2"/>
         <v>2.02150269921875E-7</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="4">
+      <c r="D14" s="13"/>
+      <c r="E14" s="1">
         <f>0.515^2</f>
         <v>0.26522499999999999</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="3">
         <f t="shared" si="3"/>
         <v>1.949647466910156E-7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="6"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="13">
+      <c r="B17" s="16"/>
+      <c r="C17" s="7">
         <f>AVERAGE(C12:C14)</f>
         <v>1.6371845020833337E-7</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="16" t="s">
+      <c r="D17" s="14"/>
+      <c r="E17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="17">
+      <c r="F17" s="16"/>
+      <c r="G17" s="8">
         <f>AVERAGE(G12:G14)</f>
         <v>1.6050523172134897E-7</v>
       </c>
     </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.995</v>
+      </c>
+      <c r="B21" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21:C23" si="4">A21*B21^6</f>
+        <v>1.7708862304687498E-7</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="1">
+        <f>0.998^2</f>
+        <v>0.996004</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" ref="G21:G23" si="5">E21*F21^6</f>
+        <v>1.7726731347656249E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="B22" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="4"/>
+        <v>2.4137569000000015E-7</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="1">
+        <f>0.796^2</f>
+        <v>0.63361600000000007</v>
+      </c>
+      <c r="F22" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="5"/>
+        <v>2.3896796749225014E-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0.435</v>
+      </c>
+      <c r="B23" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="4"/>
+        <v>3.1976497242187496E-7</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="1">
+        <f>0.6525^2</f>
+        <v>0.42575624999999995</v>
+      </c>
+      <c r="F23" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="5"/>
+        <v>3.1296996675791011E-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="16"/>
+      <c r="C26" s="7">
+        <f>AVERAGE(C21:C23)</f>
+        <v>2.4607642848958341E-7</v>
+      </c>
+      <c r="D26" s="14"/>
+      <c r="E26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="8">
+        <f>AVERAGE(G21:G23)</f>
+        <v>2.4306841590890758E-7</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="12">
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="D20:D26"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="E26:F26"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="D2:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A10:G10"/>
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed and better documented the magnets' K values
</commit_message>
<xml_diff>
--- a/Software/K Values for Multiple Magnets.xlsx
+++ b/Software/K Values for Multiple Magnets.xlsx
@@ -5,14 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pd3dlab\Documents\Github\AugmentedStethoscope\Software\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modeh\Documents\Github\AugmentedStethoscope\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Big Magnet" sheetId="2" r:id="rId1"/>
+    <sheet name="Small Magnet" sheetId="3" r:id="rId2"/>
+    <sheet name="Spherical Magnet" sheetId="4" r:id="rId3"/>
+    <sheet name="Small Magnet (with hole)" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>x</t>
   </si>
@@ -54,6 +57,24 @@
   </si>
   <si>
     <t>SPEHRICAL MAGNET</t>
+  </si>
+  <si>
+    <t>H_x</t>
+  </si>
+  <si>
+    <t>H_y</t>
+  </si>
+  <si>
+    <t>H_z</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>K-Value</t>
+  </si>
+  <si>
+    <t>SMALL MAGNET (W\HOLE)</t>
   </si>
 </sst>
 </file>
@@ -86,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,8 +120,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -335,11 +362,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -349,6 +413,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -358,22 +440,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -391,6 +469,202 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1933575"/>
+          <a:ext cx="4648200" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>73819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1933575"/>
+          <a:ext cx="4657725" cy="3493294"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1933575"/>
+          <a:ext cx="4648200" cy="3486150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1933575"/>
+          <a:ext cx="4660900" cy="3495675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -656,10 +930,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,15 +943,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -689,7 +963,7 @@
       <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
@@ -711,7 +985,7 @@
         <f t="shared" ref="C3:C5" si="0">A3*B3^6</f>
         <v>1.2209326171874999E-6</v>
       </c>
-      <c r="D3" s="13"/>
+      <c r="D3" s="10"/>
       <c r="E3" s="1">
         <f>2.61^2</f>
         <v>6.8120999999999992</v>
@@ -735,7 +1009,7 @@
         <f t="shared" si="0"/>
         <v>1.0824191098437507E-6</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="1">
         <f>1.69^2</f>
         <v>2.8560999999999996</v>
@@ -759,7 +1033,7 @@
         <f t="shared" si="0"/>
         <v>9.6297037671875006E-7</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="1">
         <f>1.13^2</f>
         <v>1.2768999999999997</v>
@@ -776,7 +1050,7 @@
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="3"/>
@@ -785,330 +1059,467 @@
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="7">
         <f>AVERAGE(C3:C5)</f>
         <v>1.0887740345833337E-6</v>
       </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="11"/>
+      <c r="E8" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="16"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="8">
         <f>AVERAGE(G3:G5)</f>
         <v>1.0760743376682291E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>0.755</v>
-      </c>
-      <c r="B12" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" ref="C12:C14" si="2">A12*B12^6</f>
-        <v>1.3437377929687499E-7</v>
-      </c>
-      <c r="D12" s="13"/>
-      <c r="E12" s="1">
-        <f>0.863^2</f>
-        <v>0.74476900000000001</v>
-      </c>
-      <c r="F12" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G12" s="3">
-        <f t="shared" ref="G12:G14" si="3">E12*F12^6</f>
-        <v>1.3255288110351561E-7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>0.41</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="2"/>
-        <v>1.5463130140625006E-7</v>
-      </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="1">
-        <f>0.639^2</f>
-        <v>0.40832099999999999</v>
-      </c>
-      <c r="F13" s="1">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="G13" s="3">
-        <f t="shared" si="3"/>
-        <v>1.5399806736951569E-7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>0.27500000000000002</v>
-      </c>
-      <c r="B14" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="C14" s="1">
-        <f t="shared" si="2"/>
-        <v>2.02150269921875E-7</v>
-      </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="1">
-        <f>0.515^2</f>
-        <v>0.26522499999999999</v>
-      </c>
-      <c r="F14" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="G14" s="3">
-        <f t="shared" si="3"/>
-        <v>1.949647466910156E-7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="16"/>
-      <c r="C17" s="7">
-        <f>AVERAGE(C12:C14)</f>
-        <v>1.6371845020833337E-7</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="8">
-        <f>AVERAGE(G12:G14)</f>
-        <v>1.6050523172134897E-7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>0.995</v>
-      </c>
-      <c r="B21" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C21" s="1">
-        <f t="shared" ref="C21:C23" si="4">A21*B21^6</f>
-        <v>1.7708862304687498E-7</v>
-      </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="1">
-        <f>0.998^2</f>
-        <v>0.996004</v>
-      </c>
-      <c r="F21" s="1">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" ref="G21:G23" si="5">E21*F21^6</f>
-        <v>1.7726731347656249E-7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="B22" s="1">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="C22" s="1">
-        <f t="shared" si="4"/>
-        <v>2.4137569000000015E-7</v>
-      </c>
-      <c r="D22" s="13"/>
-      <c r="E22" s="1">
-        <f>0.796^2</f>
-        <v>0.63361600000000007</v>
-      </c>
-      <c r="F22" s="1">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="G22" s="3">
-        <f t="shared" si="5"/>
-        <v>2.3896796749225014E-7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>0.435</v>
-      </c>
-      <c r="B23" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="C23" s="1">
-        <f t="shared" si="4"/>
-        <v>3.1976497242187496E-7</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="1">
-        <f>0.6525^2</f>
-        <v>0.42575624999999995</v>
-      </c>
-      <c r="F23" s="1">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="G23" s="3">
-        <f t="shared" si="5"/>
-        <v>3.1296996675791011E-7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="7">
-        <f>AVERAGE(C21:C23)</f>
-        <v>2.4607642848958341E-7</v>
-      </c>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="16"/>
-      <c r="G26" s="8">
-        <f>AVERAGE(G21:G23)</f>
-        <v>2.4306841590890758E-7</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D11:D17"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="D20:D26"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="E26:F26"/>
+  <mergeCells count="4">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="D2:D8"/>
+    <mergeCell ref="A8:B8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0.19</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="0">E3*F3^6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="8">
+        <f>(A3^2+B3^2+C3^2)*F3^6</f>
+        <v>1.2903442382812499E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>0.995</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <f t="shared" ref="C3:C5" si="0">A3*B3^6</f>
+        <v>1.7708862304687498E-7</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="1">
+        <f>0.998^2</f>
+        <v>0.996004</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="1">E3*F3^6</f>
+        <v>1.7726731347656249E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4137569000000015E-7</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="1">
+        <f>0.796^2</f>
+        <v>0.63361600000000007</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="1"/>
+        <v>2.3896796749225014E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>0.435</v>
+      </c>
+      <c r="B5" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1976497242187496E-7</v>
+      </c>
+      <c r="D5" s="10"/>
+      <c r="E5" s="1">
+        <f>0.6525^2</f>
+        <v>0.42575624999999995</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="1"/>
+        <v>3.1296996675791011E-7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13"/>
+      <c r="C8" s="7">
+        <f>AVERAGE(C3:C5)</f>
+        <v>2.4607642848958341E-7</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="8">
+        <f>AVERAGE(G3:G5)</f>
+        <v>2.4306841590890758E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D2:D8"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E8:F8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1.02</v>
+      </c>
+      <c r="D3" s="25"/>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3" si="0">E3*F3^6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="8">
+        <f>(A3^2+B3^2+C3^2)*F3^6</f>
+        <v>1.8691303710937498E-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="D2:D7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>